<commit_message>
Adição do botão para exibir o estoque, permitindo o usuário conferir o numero de itens antes de cautelar ou descautelar
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -1,33 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amado\Documents\VSCodeProjects\ProgAp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A2E9DF-85A7-4323-9BCE-B7D7451540DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="4836" yWindow="1308" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>Histórico</t>
+  </si>
+  <si>
+    <t>Parafuso</t>
+  </si>
+  <si>
+    <t>Martelo</t>
+  </si>
+  <si>
+    <t>Cadeado</t>
+  </si>
+  <si>
+    <t>Fardo aberto</t>
+  </si>
+  <si>
+    <t>Cantil</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,80 +80,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -385,67 +360,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col width="13.88671875" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15.88671875" customWidth="1" min="3" max="3"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Item</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Quantidade</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Histórico</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Parafuso</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-2024-11-14 21:35:08.833218 - Eduardo retirou 1
-2024-11-15 09:51:42.979103 - admin@example.com retirou 3
-2024-11-15 09:52:44.332277 - admin@example.com retirou 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Martelo</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adição da função que salva em um arquivo .txt o histórico de movimentaçõs no estoque com nome e número do usuário que retira um item
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -1,67 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amado\Documents\VSCodeProjects\ProgAp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A2E9DF-85A7-4323-9BCE-B7D7451540DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4836" yWindow="1308" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4836" yWindow="1308" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Quantidade</t>
-  </si>
-  <si>
-    <t>Histórico</t>
-  </si>
-  <si>
-    <t>Parafuso</t>
-  </si>
-  <si>
-    <t>Martelo</t>
-  </si>
-  <si>
-    <t>Cadeado</t>
-  </si>
-  <si>
-    <t>Fardo aberto</t>
-  </si>
-  <si>
-    <t>Cantil</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -80,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -360,69 +385,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col width="13.88671875" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15.88671875" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Quantidade</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Histórico</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Parafuso</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Martelo</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+2024-11-16 22:11:46.558990 - Eduardo retirou 5 </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cadeado</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Fardo aberto</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>20</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+2024-11-16 22:13:08.269940 - Morel retirou 10 </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cantil</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+2024-11-16 22:18:02.119432 - Eduardo retirou 5 
+2024-11-16 22:22:18.262439 - Eduardo retirou 5 
+2024-11-16 22:22:23.833104 - 1 devolveu 5</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge com o peixoto e ajustando algumas partes do código para a localização da planilha e das imagens
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -396,7 +396,7 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="13.88671875" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
@@ -427,7 +427,14 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>170</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+2024-11-17 16:35:26.788396 - admin@example.com devolveu 10
+2024-11-17 16:35:45.177355 - admin@example.com devolveu 150</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -437,12 +444,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">
-2024-11-16 22:11:46.558990 - Eduardo retirou 5 </t>
+2024-11-16 22:11:46.558990 - Eduardo retirou 5 
+2024-11-17 20:11:39.009979 - Morel retirou 1 </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
inventário dos usuários pronto!
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -390,10 +390,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -414,90 +414,118 @@
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Histórico</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Parafuso</t>
+          <t>Marmita</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>170</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-2024-11-17 16:35:26.788396 - admin@example.com devolveu 10
-2024-11-17 16:35:45.177355 - admin@example.com devolveu 150</t>
-        </is>
+        <v>169</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Martelo</t>
+          <t>Porta cantil</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-2024-11-16 22:11:46.558990 - Eduardo retirou 5 
-2024-11-17 20:11:39.009979 - Morel retirou 1 </t>
-        </is>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cadeado</t>
+          <t>Cantil</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Fardo aberto</t>
+          <t>Suspensório</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>20</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-2024-11-16 22:13:08.269940 - Morel retirou 10 </t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Cantil</t>
+          <t>Cinto</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>5</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-2024-11-16 22:18:02.119432 - Eduardo retirou 5 
-2024-11-16 22:22:18.262439 - Eduardo retirou 5 
-2024-11-16 22:22:23.833104 - 1 devolveu 5</t>
-        </is>
-      </c>
-    </row>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Coldre</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Meia VO</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Meia branca (TFM)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Saco VO</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Fivela preta</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Fivela dourada</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adicionando a funcionalidade do encarregado de materiais (pode adicionar e remover itens do estoque, somente)
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -442,7 +442,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>19</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5">
@@ -525,7 +525,16 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13"/>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Bandeira do Brasil</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>